<commit_message>
increasing time available to workflows
</commit_message>
<xml_diff>
--- a/test_data/norfolk_coastal_flooding/full_benchmarking_experiment_uva.xlsx
+++ b/test_data/norfolk_coastal_flooding/full_benchmarking_experiment_uva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\test_data\norfolk_coastal_flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB27ECE-0447-4999-A841-4636E84E79C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121AC361-BE68-4065-A2A1-0DE62BEFE952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4185" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -419,6 +419,74 @@
   <dxfs count="17">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -450,74 +518,6 @@
         <bottom/>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -897,20 +897,20 @@
     <tableColumn id="3" xr3:uid="{3A65E5E5-CB8B-4698-A27C-21DF3A95D49A}" name="n_mpi_procs" dataDxfId="8" dataCellStyle="Input"/>
     <tableColumn id="4" xr3:uid="{D366E835-7967-45B3-94DD-92B04C3126AA}" name="n_omp_threads" dataDxfId="7" dataCellStyle="Input"/>
     <tableColumn id="8" xr3:uid="{53D9FE6F-92F7-4A3A-B94F-6A698F029BE0}" name="n_gpus" dataDxfId="6" dataCellStyle="Input"/>
-    <tableColumn id="12" xr3:uid="{97D9BCE9-C2EB-487D-9081-3F6B6CACB117}" name="hpc_ensemble_partition" dataDxfId="1" dataCellStyle="Input"/>
-    <tableColumn id="13" xr3:uid="{96650528-E8C5-445B-8564-B12E25175139}" name="hpc_time_min_per_sim" dataDxfId="0" dataCellStyle="Input">
+    <tableColumn id="12" xr3:uid="{97D9BCE9-C2EB-487D-9081-3F6B6CACB117}" name="hpc_ensemble_partition" dataDxfId="5" dataCellStyle="Input"/>
+    <tableColumn id="13" xr3:uid="{96650528-E8C5-445B-8564-B12E25175139}" name="hpc_time_min_per_sim" dataDxfId="4" dataCellStyle="Input">
       <calculatedColumnFormula>60*6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F6B7A6B4-BD4B-4406-BCB7-C3DBCC48FA6B}" name="total_OpenMP_threads" dataDxfId="5" dataCellStyle="Output">
+    <tableColumn id="6" xr3:uid="{F6B7A6B4-BD4B-4406-BCB7-C3DBCC48FA6B}" name="total_OpenMP_threads" dataDxfId="3" dataCellStyle="Output">
       <calculatedColumnFormula>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{8B064801-C992-4C19-AF9B-73CC7D0951B1}" name="total_devices" dataDxfId="4" dataCellStyle="Output">
+    <tableColumn id="7" xr3:uid="{8B064801-C992-4C19-AF9B-73CC7D0951B1}" name="total_devices" dataDxfId="2" dataCellStyle="Output">
       <calculatedColumnFormula>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C813D3D6-6AEA-4168-A5C0-6FD56BB1D36D}" name="devices_per_node" dataDxfId="3" dataCellStyle="Output">
+    <tableColumn id="10" xr3:uid="{C813D3D6-6AEA-4168-A5C0-6FD56BB1D36D}" name="devices_per_node" dataDxfId="1" dataCellStyle="Output">
       <calculatedColumnFormula>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{47E652A1-51DD-4A45-9FB0-F72E592EF0D3}" name="check" dataDxfId="2">
+    <tableColumn id="5" xr3:uid="{47E652A1-51DD-4A45-9FB0-F72E592EF0D3}" name="check" dataDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1184,24 +1184,24 @@
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="28.33203125" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="28.28515625" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>23</v>
       </c>
       <c r="I2" s="6">
-        <f>60*6</f>
+        <f t="shared" ref="I2:I45" si="0">60*6</f>
         <v>360</v>
       </c>
       <c r="J2" s="7">
@@ -1288,7 +1288,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>23</v>
       </c>
       <c r="I3" s="6">
-        <f>60*6</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="J3" s="7">
@@ -1334,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>3</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>23</v>
       </c>
       <c r="I4" s="6">
-        <f>60*6</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="J4" s="7">
@@ -1380,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="6">
-        <f>60*6</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="J5" s="7">
@@ -1426,7 +1426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>23</v>
       </c>
       <c r="I6" s="6">
-        <f>60*6</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="J6" s="7">
@@ -1472,7 +1472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>3</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>23</v>
       </c>
       <c r="I7" s="6">
-        <f>60*6</f>
+        <f t="shared" si="0"/>
         <v>360</v>
       </c>
       <c r="J7" s="7">
@@ -1518,7 +1518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
@@ -1544,8 +1544,8 @@
         <v>23</v>
       </c>
       <c r="I8" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J8" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -1590,8 +1590,8 @@
         <v>23</v>
       </c>
       <c r="I9" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J9" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1610,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
@@ -1636,8 +1636,8 @@
         <v>23</v>
       </c>
       <c r="I10" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J10" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>3</v>
       </c>
@@ -1682,8 +1682,8 @@
         <v>23</v>
       </c>
       <c r="I11" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J11" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1702,7 +1702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>5</v>
       </c>
@@ -1728,8 +1728,8 @@
         <v>23</v>
       </c>
       <c r="I12" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J12" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1748,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
@@ -1774,8 +1774,8 @@
         <v>23</v>
       </c>
       <c r="I13" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J13" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
@@ -1820,8 +1820,8 @@
         <v>23</v>
       </c>
       <c r="I14" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J14" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1840,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>4</v>
       </c>
@@ -1866,8 +1866,8 @@
         <v>23</v>
       </c>
       <c r="I15" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J15" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>3</v>
       </c>
@@ -1912,8 +1912,8 @@
         <v>23</v>
       </c>
       <c r="I16" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J16" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1932,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
@@ -1958,8 +1958,8 @@
         <v>23</v>
       </c>
       <c r="I17" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J17" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -1978,7 +1978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
@@ -2004,8 +2004,8 @@
         <v>23</v>
       </c>
       <c r="I18" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J18" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2024,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
@@ -2050,8 +2050,8 @@
         <v>23</v>
       </c>
       <c r="I19" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J19" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
@@ -2096,8 +2096,8 @@
         <v>23</v>
       </c>
       <c r="I20" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J20" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2116,7 +2116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>4</v>
       </c>
@@ -2142,8 +2142,8 @@
         <v>23</v>
       </c>
       <c r="I21" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J21" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2162,7 +2162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>3</v>
       </c>
@@ -2188,8 +2188,8 @@
         <v>23</v>
       </c>
       <c r="I22" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J22" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2208,7 +2208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>5</v>
       </c>
@@ -2234,8 +2234,8 @@
         <v>23</v>
       </c>
       <c r="I23" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J23" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>5</v>
       </c>
@@ -2280,8 +2280,8 @@
         <v>23</v>
       </c>
       <c r="I24" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J24" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2300,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>5</v>
       </c>
@@ -2326,8 +2326,8 @@
         <v>23</v>
       </c>
       <c r="I25" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J25" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2346,7 +2346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>5</v>
       </c>
@@ -2372,8 +2372,8 @@
         <v>23</v>
       </c>
       <c r="I26" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J26" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2392,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>5</v>
       </c>
@@ -2418,8 +2418,8 @@
         <v>23</v>
       </c>
       <c r="I27" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J27" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2438,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>4</v>
       </c>
@@ -2464,8 +2464,8 @@
         <v>23</v>
       </c>
       <c r="I28" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J28" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2484,7 +2484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>3</v>
       </c>
@@ -2510,8 +2510,8 @@
         <v>23</v>
       </c>
       <c r="I29" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J29" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2530,7 +2530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>5</v>
       </c>
@@ -2556,8 +2556,8 @@
         <v>24</v>
       </c>
       <c r="I30" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J30" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2576,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>5</v>
       </c>
@@ -2602,8 +2602,8 @@
         <v>24</v>
       </c>
       <c r="I31" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J31" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>5</v>
       </c>
@@ -2648,8 +2648,8 @@
         <v>24</v>
       </c>
       <c r="I32" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J32" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2668,7 +2668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>5</v>
       </c>
@@ -2694,8 +2694,8 @@
         <v>24</v>
       </c>
       <c r="I33" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J33" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2714,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>5</v>
       </c>
@@ -2740,8 +2740,8 @@
         <v>24</v>
       </c>
       <c r="I34" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J34" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2760,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>5</v>
       </c>
@@ -2786,8 +2786,8 @@
         <v>24</v>
       </c>
       <c r="I35" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J35" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2806,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>4</v>
       </c>
@@ -2832,8 +2832,8 @@
         <v>24</v>
       </c>
       <c r="I36" s="6">
-        <f>60*2</f>
-        <v>120</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J36" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2852,7 +2852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>1</v>
       </c>
@@ -2878,7 +2878,8 @@
         <v>20</v>
       </c>
       <c r="I37" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J37" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2897,7 +2898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>1</v>
       </c>
@@ -2923,7 +2924,8 @@
         <v>20</v>
       </c>
       <c r="I38" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J38" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2942,7 +2944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>1</v>
       </c>
@@ -2968,7 +2970,8 @@
         <v>20</v>
       </c>
       <c r="I39" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J39" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -2987,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>1</v>
       </c>
@@ -3013,7 +3016,8 @@
         <v>20</v>
       </c>
       <c r="I40" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J40" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -3032,7 +3036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>1</v>
       </c>
@@ -3058,7 +3062,8 @@
         <v>20</v>
       </c>
       <c r="I41" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J41" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -3077,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>1</v>
       </c>
@@ -3103,7 +3108,8 @@
         <v>20</v>
       </c>
       <c r="I42" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J42" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -3122,7 +3128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>1</v>
       </c>
@@ -3148,7 +3154,8 @@
         <v>20</v>
       </c>
       <c r="I43" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J43" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -3167,7 +3174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>1</v>
       </c>
@@ -3193,7 +3200,8 @@
         <v>20</v>
       </c>
       <c r="I44" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J44" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
@@ -3212,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>1</v>
       </c>
@@ -3238,7 +3246,8 @@
         <v>20</v>
       </c>
       <c r="I45" s="6">
-        <v>60</v>
+        <f t="shared" si="0"/>
+        <v>360</v>
       </c>
       <c r="J45" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>

</xml_diff>

<commit_message>
remove some pointless jobs
</commit_message>
<xml_diff>
--- a/test_data/norfolk_coastal_flooding/full_benchmarking_experiment_uva.xlsx
+++ b/test_data/norfolk_coastal_flooding/full_benchmarking_experiment_uva.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dcl3nd\dev\TRITON-SWMM_toolkit\test_data\norfolk_coastal_flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121AC361-BE68-4065-A2A1-0DE62BEFE952}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC1706-A6F6-4C79-AC9C-10CF32F9C760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="26">
   <si>
     <t>CPU</t>
   </si>
@@ -884,10 +884,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}" name="Table1" displayName="Table1" ref="A1:M45" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:M45" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M45">
-    <sortCondition ref="B1:B45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}" name="Table1" displayName="Table1" ref="A1:M42" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
+  <autoFilter ref="A1:M42" xr:uid="{1A4495C6-64F1-4654-82C3-1417CFDBC1D1}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M42">
+    <sortCondition ref="C1:C42"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="11" xr3:uid="{3DECB62C-AAF2-4EC7-8598-5E8776D4B845}" name="hardware_utilization_strategy" dataDxfId="12" dataCellStyle="Note"/>
@@ -1181,10 +1181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1243,409 +1243,409 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>0</v>
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J2" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>1</v>
+      </c>
+      <c r="L2" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+      <c r="M2" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>2</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J3" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>2</v>
+      </c>
+      <c r="K3" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>2</v>
+      </c>
+      <c r="L3" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="M3" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>3</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J4" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>3</v>
+      </c>
+      <c r="K4" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>3</v>
+      </c>
+      <c r="L4" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>3</v>
+      </c>
+      <c r="M4" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>4</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J5" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>4</v>
+      </c>
+      <c r="K5" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>4</v>
+      </c>
+      <c r="L5" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="M5" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J6" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>5</v>
+      </c>
+      <c r="K6" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>5</v>
+      </c>
+      <c r="L6" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>5</v>
+      </c>
+      <c r="M6" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1</v>
+      </c>
+      <c r="E7" s="6">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6">
+        <v>6</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J7" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>6</v>
+      </c>
+      <c r="K7" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>6</v>
+      </c>
+      <c r="L7" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>6</v>
+      </c>
+      <c r="M7" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="6">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6">
+        <v>7</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J8" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>7</v>
+      </c>
+      <c r="K8" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>7</v>
+      </c>
+      <c r="L8" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>7</v>
+      </c>
+      <c r="M8" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="6">
+        <v>8</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
+      <c r="G9" s="6">
+        <v>8</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J9" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="K9" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>8</v>
+      </c>
+      <c r="L9" s="8">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="M9" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
         <v>16</v>
       </c>
-      <c r="D2" s="12">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12">
-        <v>1</v>
-      </c>
-      <c r="F2" s="12">
-        <v>1</v>
-      </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="6">
-        <f t="shared" ref="I2:I45" si="0">60*6</f>
-        <v>360</v>
-      </c>
-      <c r="J2" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>1</v>
-      </c>
-      <c r="K2" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>1</v>
-      </c>
-      <c r="L2" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="M2" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12">
-        <v>2</v>
-      </c>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J3" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>2</v>
-      </c>
-      <c r="K3" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>2</v>
-      </c>
-      <c r="L3" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>2</v>
-      </c>
-      <c r="M3" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12">
-        <v>1</v>
-      </c>
-      <c r="F4" s="12">
-        <v>2</v>
-      </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J4" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>2</v>
-      </c>
-      <c r="K4" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>2</v>
-      </c>
-      <c r="L4" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>2</v>
-      </c>
-      <c r="M4" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="12">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12">
-        <v>2</v>
-      </c>
-      <c r="F5" s="12">
-        <v>2</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J5" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
-      </c>
-      <c r="K5" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
-      </c>
-      <c r="L5" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="M5" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12">
-        <v>4</v>
-      </c>
-      <c r="F6" s="12">
-        <v>1</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J6" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
-      </c>
-      <c r="K6" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
-      </c>
-      <c r="L6" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="M6" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="12">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12">
-        <v>1</v>
-      </c>
-      <c r="F7" s="12">
-        <v>4</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J7" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
-      </c>
-      <c r="K7" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
-      </c>
-      <c r="L7" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="M7" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="12">
-        <v>1</v>
-      </c>
-      <c r="E8" s="12">
-        <v>2</v>
-      </c>
-      <c r="F8" s="12">
-        <v>4</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J8" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
-      </c>
-      <c r="K8" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
-      </c>
-      <c r="L8" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="M8" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="12">
-        <v>1</v>
-      </c>
-      <c r="E9" s="12">
-        <v>4</v>
-      </c>
-      <c r="F9" s="12">
-        <v>2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J9" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
-      </c>
-      <c r="K9" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
-      </c>
-      <c r="L9" s="8">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="M9" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="12">
-        <v>1</v>
-      </c>
-      <c r="E10" s="12">
-        <v>8</v>
-      </c>
-      <c r="F10" s="12">
+      <c r="F10" s="6">
         <v>1</v>
       </c>
       <c r="G10" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J10" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="K10" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L10" s="8">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
@@ -1658,22 +1658,22 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="12">
         <v>1</v>
       </c>
       <c r="E11" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G11" s="6">
         <v>0</v>
@@ -1682,20 +1682,20 @@
         <v>23</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J11" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K11" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L11" s="8">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M11" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -1716,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" s="13">
         <v>4</v>
@@ -1728,20 +1728,20 @@
         <v>23</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J12" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K12" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L12" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M12" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -1762,10 +1762,10 @@
         <v>1</v>
       </c>
       <c r="E13" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" s="12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G13" s="6">
         <v>0</v>
@@ -1774,20 +1774,20 @@
         <v>23</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J13" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K13" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="L13" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="M13" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -1808,10 +1808,10 @@
         <v>1</v>
       </c>
       <c r="E14" s="12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F14" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G14" s="6">
         <v>0</v>
@@ -1820,7 +1820,7 @@
         <v>23</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J14" s="7">
@@ -1842,22 +1842,22 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="12">
         <v>1</v>
       </c>
       <c r="E15" s="12">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="F15" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G15" s="6">
         <v>0</v>
@@ -1866,7 +1866,7 @@
         <v>23</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J15" s="7">
@@ -1888,22 +1888,22 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D16" s="12">
         <v>1</v>
       </c>
       <c r="E16" s="12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F16" s="12">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="G16" s="6">
         <v>0</v>
@@ -1912,7 +1912,7 @@
         <v>23</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J16" s="7">
@@ -1958,7 +1958,7 @@
         <v>23</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J17" s="7">
@@ -2004,7 +2004,7 @@
         <v>23</v>
       </c>
       <c r="I18" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J18" s="7">
@@ -2050,7 +2050,7 @@
         <v>23</v>
       </c>
       <c r="I19" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J19" s="7">
@@ -2096,7 +2096,7 @@
         <v>23</v>
       </c>
       <c r="I20" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J20" s="7">
@@ -2118,22 +2118,22 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="12">
         <v>1</v>
       </c>
       <c r="E21" s="12">
+        <v>2</v>
+      </c>
+      <c r="F21" s="12">
         <v>32</v>
-      </c>
-      <c r="F21" s="12">
-        <v>1</v>
       </c>
       <c r="G21" s="6">
         <v>0</v>
@@ -2142,20 +2142,20 @@
         <v>23</v>
       </c>
       <c r="I21" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J21" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="K21" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L21" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="M21" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -2164,22 +2164,22 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D22" s="12">
         <v>1</v>
       </c>
       <c r="E22" s="12">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="F22" s="12">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="G22" s="6">
         <v>0</v>
@@ -2188,20 +2188,20 @@
         <v>23</v>
       </c>
       <c r="I22" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J22" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="K22" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="L22" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="M22" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -2222,10 +2222,10 @@
         <v>1</v>
       </c>
       <c r="E23" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F23" s="12">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -2234,7 +2234,7 @@
         <v>23</v>
       </c>
       <c r="I23" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J23" s="7">
@@ -2268,10 +2268,10 @@
         <v>1</v>
       </c>
       <c r="E24" s="12">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="F24" s="12">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G24" s="6">
         <v>0</v>
@@ -2280,7 +2280,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J24" s="7">
@@ -2314,10 +2314,10 @@
         <v>1</v>
       </c>
       <c r="E25" s="12">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F25" s="12">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G25" s="6">
         <v>0</v>
@@ -2326,7 +2326,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J25" s="7">
@@ -2356,32 +2356,32 @@
       <c r="C26" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="12">
-        <v>1</v>
-      </c>
-      <c r="E26" s="12">
-        <v>16</v>
-      </c>
-      <c r="F26" s="12">
-        <v>4</v>
-      </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>23</v>
+      <c r="D26" s="6">
+        <v>2</v>
+      </c>
+      <c r="E26" s="6">
+        <v>2</v>
+      </c>
+      <c r="F26" s="6">
+        <v>64</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="I26" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J26" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="K26" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="L26" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
@@ -2403,31 +2403,31 @@
         <v>17</v>
       </c>
       <c r="D27" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" s="12">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F27" s="12">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G27" s="6">
         <v>0</v>
       </c>
-      <c r="H27" s="6" t="s">
-        <v>23</v>
+      <c r="H27" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="I27" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J27" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="K27" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="L27" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
@@ -2440,40 +2440,40 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D28" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="12">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="F28" s="12">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="G28" s="6">
         <v>0</v>
       </c>
-      <c r="H28" s="6" t="s">
-        <v>23</v>
+      <c r="H28" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="I28" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J28" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="K28" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="L28" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
@@ -2486,40 +2486,40 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D29" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E29" s="12">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F29" s="12">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="G29" s="6">
         <v>0</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>23</v>
+      <c r="H29" s="18" t="s">
+        <v>24</v>
       </c>
       <c r="I29" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J29" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="K29" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="L29" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
@@ -2540,23 +2540,23 @@
       <c r="C30" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="6">
-        <v>2</v>
-      </c>
-      <c r="E30" s="6">
-        <v>2</v>
-      </c>
-      <c r="F30" s="6">
-        <v>64</v>
-      </c>
-      <c r="G30" s="18">
+      <c r="D30" s="12">
+        <v>2</v>
+      </c>
+      <c r="E30" s="12">
+        <v>32</v>
+      </c>
+      <c r="F30" s="12">
+        <v>4</v>
+      </c>
+      <c r="G30" s="6">
         <v>0</v>
       </c>
       <c r="H30" s="18" t="s">
         <v>24</v>
       </c>
       <c r="I30" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J30" s="7">
@@ -2589,20 +2589,20 @@
       <c r="D31" s="12">
         <v>2</v>
       </c>
-      <c r="E31" s="12">
-        <v>4</v>
-      </c>
-      <c r="F31" s="12">
-        <v>32</v>
-      </c>
-      <c r="G31" s="6">
+      <c r="E31" s="6">
+        <v>64</v>
+      </c>
+      <c r="F31" s="6">
+        <v>2</v>
+      </c>
+      <c r="G31" s="18">
         <v>0</v>
       </c>
       <c r="H31" s="18" t="s">
         <v>24</v>
       </c>
       <c r="I31" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J31" s="7">
@@ -2624,44 +2624,44 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E32" s="12">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F32" s="12">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="G32" s="6">
         <v>0</v>
       </c>
-      <c r="H32" s="18" t="s">
-        <v>24</v>
+      <c r="H32" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I32" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J32" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="K32" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="L32" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
+        <v>2</v>
       </c>
       <c r="M32" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -2670,44 +2670,44 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D33" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="12">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F33" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G33" s="6">
         <v>0</v>
       </c>
-      <c r="H33" s="18" t="s">
-        <v>24</v>
+      <c r="H33" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I33" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J33" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="K33" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>4</v>
       </c>
       <c r="L33" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="M33" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -2716,44 +2716,44 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D34" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="12">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F34" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G34" s="6">
         <v>0</v>
       </c>
-      <c r="H34" s="18" t="s">
-        <v>24</v>
+      <c r="H34" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I34" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J34" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="K34" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="L34" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="M34" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -2762,44 +2762,44 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D35" s="12">
-        <v>2</v>
-      </c>
-      <c r="E35" s="6">
-        <v>64</v>
-      </c>
-      <c r="F35" s="6">
-        <v>2</v>
-      </c>
-      <c r="G35" s="18">
-        <v>0</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="E35" s="12">
+        <v>16</v>
+      </c>
+      <c r="F35" s="12">
+        <v>1</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="I35" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J35" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="K35" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
+        <v>16</v>
       </c>
       <c r="L35" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="M35" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -2808,274 +2808,274 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="12">
+        <v>1</v>
+      </c>
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="12">
+        <v>2</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I36" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J36" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>2</v>
+      </c>
+      <c r="K36" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>2</v>
+      </c>
+      <c r="L36" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>2</v>
+      </c>
+      <c r="M36" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="12">
+        <v>1</v>
+      </c>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="12">
         <v>4</v>
       </c>
-      <c r="B36" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="12">
-        <v>2</v>
-      </c>
-      <c r="E36" s="12">
-        <v>128</v>
-      </c>
-      <c r="F36" s="12">
-        <v>1</v>
-      </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="I36" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J36" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>128</v>
-      </c>
-      <c r="K36" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>128</v>
-      </c>
-      <c r="L36" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I37" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J37" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>4</v>
+      </c>
+      <c r="K37" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>4</v>
+      </c>
+      <c r="L37" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>4</v>
+      </c>
+      <c r="M37" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="12">
+        <v>1</v>
+      </c>
+      <c r="E38" s="12">
+        <v>1</v>
+      </c>
+      <c r="F38" s="12">
+        <v>8</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I38" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J38" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>8</v>
+      </c>
+      <c r="K38" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>8</v>
+      </c>
+      <c r="L38" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>8</v>
+      </c>
+      <c r="M38" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="12">
+        <v>1</v>
+      </c>
+      <c r="E39" s="12">
+        <v>1</v>
+      </c>
+      <c r="F39" s="12">
+        <v>16</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I39" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J39" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>16</v>
+      </c>
+      <c r="K39" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>16</v>
+      </c>
+      <c r="L39" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>16</v>
+      </c>
+      <c r="M39" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="12">
+        <v>1</v>
+      </c>
+      <c r="E40" s="12">
+        <v>1</v>
+      </c>
+      <c r="F40" s="12">
+        <v>32</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I40" s="6">
+        <f>60*6</f>
+        <v>360</v>
+      </c>
+      <c r="J40" s="7">
+        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
+        <v>32</v>
+      </c>
+      <c r="K40" s="7">
+        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
+        <v>32</v>
+      </c>
+      <c r="L40" s="9">
+        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
+        <v>32</v>
+      </c>
+      <c r="M40" t="b">
+        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="12">
+        <v>1</v>
+      </c>
+      <c r="E41" s="12">
+        <v>1</v>
+      </c>
+      <c r="F41" s="12">
         <v>64</v>
       </c>
-      <c r="M36" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D37" s="6">
-        <v>1</v>
-      </c>
-      <c r="E37" s="6">
-        <v>1</v>
-      </c>
-      <c r="F37" s="6">
-        <v>1</v>
-      </c>
-      <c r="G37" s="6">
-        <v>1</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I37" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J37" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>1</v>
-      </c>
-      <c r="K37" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>1</v>
-      </c>
-      <c r="L37" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-      <c r="M37" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D38" s="6">
-        <v>1</v>
-      </c>
-      <c r="E38" s="6">
-        <v>2</v>
-      </c>
-      <c r="F38" s="6">
-        <v>1</v>
-      </c>
-      <c r="G38" s="6">
-        <v>2</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I38" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J38" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>2</v>
-      </c>
-      <c r="K38" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>2</v>
-      </c>
-      <c r="L38" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>2</v>
-      </c>
-      <c r="M38" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D39" s="6">
-        <v>1</v>
-      </c>
-      <c r="E39" s="6">
-        <v>3</v>
-      </c>
-      <c r="F39" s="6">
-        <v>1</v>
-      </c>
-      <c r="G39" s="6">
-        <v>3</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I39" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J39" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>3</v>
-      </c>
-      <c r="K39" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>3</v>
-      </c>
-      <c r="L39" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>3</v>
-      </c>
-      <c r="M39" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="6">
-        <v>1</v>
-      </c>
-      <c r="E40" s="6">
-        <v>4</v>
-      </c>
-      <c r="F40" s="6">
-        <v>1</v>
-      </c>
-      <c r="G40" s="6">
-        <v>4</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I40" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J40" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>4</v>
-      </c>
-      <c r="K40" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>4</v>
-      </c>
-      <c r="L40" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>4</v>
-      </c>
-      <c r="M40" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D41" s="6">
-        <v>1</v>
-      </c>
-      <c r="E41" s="6">
-        <v>5</v>
-      </c>
-      <c r="F41" s="6">
-        <v>1</v>
-      </c>
       <c r="G41" s="6">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I41" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J41" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="K41" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="L41" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="M41" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
@@ -3083,185 +3083,47 @@
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>1</v>
+      <c r="A42" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>0</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="6">
-        <v>1</v>
-      </c>
-      <c r="E42" s="6">
-        <v>6</v>
-      </c>
-      <c r="F42" s="6">
+        <v>16</v>
+      </c>
+      <c r="D42" s="12">
+        <v>1</v>
+      </c>
+      <c r="E42" s="12">
+        <v>1</v>
+      </c>
+      <c r="F42" s="12">
         <v>1</v>
       </c>
       <c r="G42" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I42" s="6">
-        <f t="shared" si="0"/>
+        <f>60*6</f>
         <v>360</v>
       </c>
       <c r="J42" s="7">
         <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K42" s="7">
         <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="L42" s="9">
         <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="M42" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D43" s="6">
-        <v>1</v>
-      </c>
-      <c r="E43" s="6">
-        <v>7</v>
-      </c>
-      <c r="F43" s="6">
-        <v>1</v>
-      </c>
-      <c r="G43" s="6">
-        <v>7</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I43" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J43" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>7</v>
-      </c>
-      <c r="K43" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>7</v>
-      </c>
-      <c r="L43" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>7</v>
-      </c>
-      <c r="M43" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D44" s="6">
-        <v>1</v>
-      </c>
-      <c r="E44" s="6">
-        <v>8</v>
-      </c>
-      <c r="F44" s="6">
-        <v>1</v>
-      </c>
-      <c r="G44" s="6">
-        <v>8</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I44" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J44" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>8</v>
-      </c>
-      <c r="K44" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>8</v>
-      </c>
-      <c r="L44" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="M44" t="b">
-        <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D45" s="6">
-        <v>2</v>
-      </c>
-      <c r="E45" s="6">
-        <v>16</v>
-      </c>
-      <c r="F45" s="6">
-        <v>1</v>
-      </c>
-      <c r="G45" s="6">
-        <v>16</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I45" s="6">
-        <f t="shared" si="0"/>
-        <v>360</v>
-      </c>
-      <c r="J45" s="7">
-        <f>Table1[[#This Row],[n_mpi_procs]]*Table1[[#This Row],[n_omp_threads]]</f>
-        <v>16</v>
-      </c>
-      <c r="K45" s="7">
-        <f>Table1[[#This Row],[n_omp_threads]]*Table1[[#This Row],[n_mpi_procs]]</f>
-        <v>16</v>
-      </c>
-      <c r="L45" s="9">
-        <f>Table1[[#This Row],[total_devices]]/Table1[[#This Row],[n_nodes]]</f>
-        <v>8</v>
-      </c>
-      <c r="M45" t="b">
         <f>Table1[[#This Row],[n_mpi_procs]]&gt;=Table1[[#This Row],[n_nodes]]</f>
         <v>1</v>
       </c>

</xml_diff>